<commit_message>
worked on finding the max errors with the cdc.
git-svn-id: https://forge.cornell.edu/svn/repos/automated_design@3530 d22a8b0d-b447-0410-a14f-ca4c0a428a39
</commit_message>
<xml_diff>
--- a/Final Designs/April 10 2011 CDC experimental results.xlsx
+++ b/Final Designs/April 10 2011 CDC experimental results.xlsx
@@ -13,7 +13,6 @@
     <sheet name="15-Mar-11" sheetId="5" r:id="rId4"/>
     <sheet name="10-Apr-11" sheetId="7" r:id="rId5"/>
     <sheet name="10-Apr-11 (2)" sheetId="8" r:id="rId6"/>
-    <sheet name="MaxError" sheetId="9" r:id="rId7"/>
   </sheets>
   <definedNames>
     <definedName name="solver_adj" localSheetId="4" hidden="1">'10-Apr-11'!$N$7</definedName>
@@ -124,7 +123,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="36">
   <si>
     <t>AguaClara Lab</t>
   </si>
@@ -216,12 +215,6 @@
     <t>Notes: L = 9.675ft. D = 0.124in</t>
   </si>
   <si>
-    <t>Qexpected</t>
-  </si>
-  <si>
-    <t>Qlinear</t>
-  </si>
-  <si>
     <t>Error</t>
   </si>
   <si>
@@ -232,6 +225,12 @@
   </si>
   <si>
     <t>actual</t>
+  </si>
+  <si>
+    <t>Actual</t>
+  </si>
+  <si>
+    <t>Expected</t>
   </si>
 </sst>
 </file>
@@ -316,7 +315,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="43">
+  <cellXfs count="46">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="15" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
@@ -418,6 +417,11 @@
     <xf numFmtId="165" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -620,7 +624,7 @@
             <c:trendlineLbl>
               <c:layout>
                 <c:manualLayout>
-                  <c:x val="-0.25306903661170954"/>
+                  <c:x val="-0.25306903661170949"/>
                   <c:y val="0.19848075146114294"/>
                 </c:manualLayout>
               </c:layout>
@@ -914,12 +918,11 @@
             </c:numRef>
           </c:yVal>
         </c:ser>
-        <c:dLbls/>
-        <c:axId val="66190720"/>
-        <c:axId val="66725376"/>
+        <c:axId val="78632064"/>
+        <c:axId val="78633984"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="66190720"/>
+        <c:axId val="78632064"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -944,12 +947,12 @@
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="66725376"/>
+        <c:crossAx val="78633984"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="66725376"/>
+        <c:axId val="78633984"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -975,7 +978,7 @@
         <c:numFmt formatCode="0.00" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="66190720"/>
+        <c:crossAx val="78632064"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -988,7 +991,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000155" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000155" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000167" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000167" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -1182,8 +1185,8 @@
             <c:trendlineLbl>
               <c:layout>
                 <c:manualLayout>
-                  <c:x val="-0.15596279017401682"/>
-                  <c:y val="0.17659654314269083"/>
+                  <c:x val="-0.15596279017401687"/>
+                  <c:y val="0.17659654314269088"/>
                 </c:manualLayout>
               </c:layout>
               <c:numFmt formatCode="General" sourceLinked="0"/>
@@ -1476,12 +1479,11 @@
             </c:numRef>
           </c:yVal>
         </c:ser>
-        <c:dLbls/>
-        <c:axId val="67168512"/>
-        <c:axId val="68252032"/>
+        <c:axId val="81416192"/>
+        <c:axId val="81418112"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="67168512"/>
+        <c:axId val="81416192"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1506,12 +1508,12 @@
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="68252032"/>
+        <c:crossAx val="81418112"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="68252032"/>
+        <c:axId val="81418112"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1537,7 +1539,7 @@
         <c:numFmt formatCode="0.00" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="67168512"/>
+        <c:crossAx val="81416192"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1550,7 +1552,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.750000000000002" l="0.70000000000000062" r="0.70000000000000062" t="0.750000000000002" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000211" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000211" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -1699,7 +1701,7 @@
             <c:trendlineLbl>
               <c:layout>
                 <c:manualLayout>
-                  <c:x val="-0.25306903661170904"/>
+                  <c:x val="-0.25306903661170899"/>
                   <c:y val="0.19848075146114294"/>
                 </c:manualLayout>
               </c:layout>
@@ -1948,12 +1950,11 @@
             </c:numRef>
           </c:yVal>
         </c:ser>
-        <c:dLbls/>
-        <c:axId val="68600960"/>
-        <c:axId val="68602880"/>
+        <c:axId val="81500800"/>
+        <c:axId val="81662720"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="68600960"/>
+        <c:axId val="81500800"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1978,12 +1979,12 @@
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="68602880"/>
+        <c:crossAx val="81662720"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="68602880"/>
+        <c:axId val="81662720"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="0"/>
@@ -2010,7 +2011,7 @@
         <c:numFmt formatCode="0.00" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="68600960"/>
+        <c:crossAx val="81500800"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2023,7 +2024,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000244" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000244" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000255" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000255" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -2172,7 +2173,7 @@
             <c:trendlineLbl>
               <c:layout>
                 <c:manualLayout>
-                  <c:x val="-0.25306903661170915"/>
+                  <c:x val="-0.2530690366117091"/>
                   <c:y val="0.19848075146114294"/>
                 </c:manualLayout>
               </c:layout>
@@ -2421,12 +2422,11 @@
             </c:numRef>
           </c:yVal>
         </c:ser>
-        <c:dLbls/>
-        <c:axId val="73572352"/>
-        <c:axId val="73574272"/>
+        <c:axId val="87844352"/>
+        <c:axId val="87846272"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="73572352"/>
+        <c:axId val="87844352"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2451,12 +2451,12 @@
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="73574272"/>
+        <c:crossAx val="87846272"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="73574272"/>
+        <c:axId val="87846272"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2482,7 +2482,7 @@
         <c:numFmt formatCode="0.00" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="73572352"/>
+        <c:crossAx val="87844352"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2495,7 +2495,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000222" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000222" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000233" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000233" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -2535,9 +2535,9 @@
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
           <c:x val="0.13012079498646364"/>
-          <c:y val="0.15973703047884572"/>
-          <c:w val="0.55139092591966765"/>
-          <c:h val="0.69453440329528182"/>
+          <c:y val="0.15973703047884577"/>
+          <c:w val="0.80736261108027962"/>
+          <c:h val="0.74522083908225079"/>
         </c:manualLayout>
       </c:layout>
       <c:scatterChart>
@@ -2546,86 +2546,75 @@
           <c:idx val="0"/>
           <c:order val="0"/>
           <c:tx>
-            <c:v>Actual Flow Rate</c:v>
+            <c:v>Actual</c:v>
           </c:tx>
-          <c:trendline>
-            <c:trendlineType val="linear"/>
-            <c:dispRSqr val="1"/>
-            <c:dispEq val="1"/>
-            <c:trendlineLbl>
-              <c:layout>
-                <c:manualLayout>
-                  <c:x val="-0.11048960081706521"/>
-                  <c:y val="5.9498423941026536E-2"/>
-                </c:manualLayout>
-              </c:layout>
-              <c:numFmt formatCode="General" sourceLinked="0"/>
-            </c:trendlineLbl>
-          </c:trendline>
           <c:xVal>
             <c:numRef>
-              <c:f>'10-Apr-11'!$A$7:$A$26</c:f>
+              <c:f>'10-Apr-11'!$A$6:$A$26</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="20"/>
+                <c:ptCount val="21"/>
                 <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
                   <c:v>1</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="2">
                   <c:v>2</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="3">
                   <c:v>3</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="4">
                   <c:v>4</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="5">
                   <c:v>5</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="6">
                   <c:v>6</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="7">
                   <c:v>7</c:v>
                 </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="8">
                   <c:v>8</c:v>
                 </c:pt>
-                <c:pt idx="8">
+                <c:pt idx="9">
                   <c:v>9</c:v>
                 </c:pt>
-                <c:pt idx="9">
+                <c:pt idx="10">
                   <c:v>10</c:v>
                 </c:pt>
-                <c:pt idx="10">
+                <c:pt idx="11">
                   <c:v>11</c:v>
                 </c:pt>
-                <c:pt idx="11">
+                <c:pt idx="12">
                   <c:v>12</c:v>
                 </c:pt>
-                <c:pt idx="12">
+                <c:pt idx="13">
                   <c:v>13</c:v>
                 </c:pt>
-                <c:pt idx="13">
+                <c:pt idx="14">
                   <c:v>14</c:v>
                 </c:pt>
-                <c:pt idx="14">
+                <c:pt idx="15">
                   <c:v>15</c:v>
                 </c:pt>
-                <c:pt idx="15">
+                <c:pt idx="16">
                   <c:v>16</c:v>
                 </c:pt>
-                <c:pt idx="16">
+                <c:pt idx="17">
                   <c:v>17</c:v>
                 </c:pt>
-                <c:pt idx="17">
+                <c:pt idx="18">
                   <c:v>18</c:v>
                 </c:pt>
-                <c:pt idx="18">
+                <c:pt idx="19">
                   <c:v>19</c:v>
                 </c:pt>
-                <c:pt idx="19">
+                <c:pt idx="20">
                   <c:v>20</c:v>
                 </c:pt>
               </c:numCache>
@@ -2633,23 +2622,26 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'10-Apr-11'!$L$7:$L$26</c:f>
+              <c:f>'10-Apr-11'!$L$6:$L$26</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
-                <c:ptCount val="20"/>
-                <c:pt idx="3">
+                <c:ptCount val="21"/>
+                <c:pt idx="0" formatCode="General">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="4">
                   <c:v>0.31111111111111112</c:v>
                 </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="8">
                   <c:v>0.6166666666666667</c:v>
                 </c:pt>
-                <c:pt idx="11">
+                <c:pt idx="12">
                   <c:v>0.90555555555555556</c:v>
                 </c:pt>
-                <c:pt idx="15">
+                <c:pt idx="16">
                   <c:v>1.1555555555555554</c:v>
                 </c:pt>
-                <c:pt idx="19">
+                <c:pt idx="20">
                   <c:v>1.3888888888888888</c:v>
                 </c:pt>
               </c:numCache>
@@ -2660,72 +2652,75 @@
           <c:idx val="1"/>
           <c:order val="1"/>
           <c:tx>
-            <c:v>Expected Flow Rate</c:v>
+            <c:v>Expected</c:v>
           </c:tx>
           <c:xVal>
             <c:numRef>
-              <c:f>'10-Apr-11'!$A$7:$A$26</c:f>
+              <c:f>'10-Apr-11'!$A$6:$A$26</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="20"/>
+                <c:ptCount val="21"/>
                 <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
                   <c:v>1</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="2">
                   <c:v>2</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="3">
                   <c:v>3</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="4">
                   <c:v>4</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="5">
                   <c:v>5</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="6">
                   <c:v>6</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="7">
                   <c:v>7</c:v>
                 </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="8">
                   <c:v>8</c:v>
                 </c:pt>
-                <c:pt idx="8">
+                <c:pt idx="9">
                   <c:v>9</c:v>
                 </c:pt>
-                <c:pt idx="9">
+                <c:pt idx="10">
                   <c:v>10</c:v>
                 </c:pt>
-                <c:pt idx="10">
+                <c:pt idx="11">
                   <c:v>11</c:v>
                 </c:pt>
-                <c:pt idx="11">
+                <c:pt idx="12">
                   <c:v>12</c:v>
                 </c:pt>
-                <c:pt idx="12">
+                <c:pt idx="13">
                   <c:v>13</c:v>
                 </c:pt>
-                <c:pt idx="13">
+                <c:pt idx="14">
                   <c:v>14</c:v>
                 </c:pt>
-                <c:pt idx="14">
+                <c:pt idx="15">
                   <c:v>15</c:v>
                 </c:pt>
-                <c:pt idx="15">
+                <c:pt idx="16">
                   <c:v>16</c:v>
                 </c:pt>
-                <c:pt idx="16">
+                <c:pt idx="17">
                   <c:v>17</c:v>
                 </c:pt>
-                <c:pt idx="17">
+                <c:pt idx="18">
                   <c:v>18</c:v>
                 </c:pt>
-                <c:pt idx="18">
+                <c:pt idx="19">
                   <c:v>19</c:v>
                 </c:pt>
-                <c:pt idx="19">
+                <c:pt idx="20">
                   <c:v>20</c:v>
                 </c:pt>
               </c:numCache>
@@ -2733,23 +2728,26 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'10-Apr-11'!$D$7:$D$26</c:f>
+              <c:f>'10-Apr-11'!$D$6:$D$26</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="20"/>
-                <c:pt idx="3">
+                <c:ptCount val="21"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="4">
                   <c:v>0.316</c:v>
                 </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="8">
                   <c:v>0.623</c:v>
                 </c:pt>
-                <c:pt idx="11">
+                <c:pt idx="12">
                   <c:v>0.92300000000000004</c:v>
                 </c:pt>
-                <c:pt idx="15">
+                <c:pt idx="16">
                   <c:v>1.2150000000000001</c:v>
                 </c:pt>
-                <c:pt idx="19">
+                <c:pt idx="20">
                   <c:v>1.5</c:v>
                 </c:pt>
               </c:numCache>
@@ -2760,75 +2758,75 @@
           <c:idx val="2"/>
           <c:order val="2"/>
           <c:tx>
-            <c:v>Expected w/Multiplier</c:v>
+            <c:v>Linear</c:v>
           </c:tx>
-          <c:trendline>
-            <c:trendlineType val="linear"/>
-          </c:trendline>
           <c:xVal>
             <c:numRef>
-              <c:f>'10-Apr-11'!$A$7:$A$26</c:f>
+              <c:f>'10-Apr-11'!$A$6:$A$26</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="20"/>
+                <c:ptCount val="21"/>
                 <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
                   <c:v>1</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="2">
                   <c:v>2</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="3">
                   <c:v>3</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="4">
                   <c:v>4</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="5">
                   <c:v>5</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="6">
                   <c:v>6</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="7">
                   <c:v>7</c:v>
                 </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="8">
                   <c:v>8</c:v>
                 </c:pt>
-                <c:pt idx="8">
+                <c:pt idx="9">
                   <c:v>9</c:v>
                 </c:pt>
-                <c:pt idx="9">
+                <c:pt idx="10">
                   <c:v>10</c:v>
                 </c:pt>
-                <c:pt idx="10">
+                <c:pt idx="11">
                   <c:v>11</c:v>
                 </c:pt>
-                <c:pt idx="11">
+                <c:pt idx="12">
                   <c:v>12</c:v>
                 </c:pt>
-                <c:pt idx="12">
+                <c:pt idx="13">
                   <c:v>13</c:v>
                 </c:pt>
-                <c:pt idx="13">
+                <c:pt idx="14">
                   <c:v>14</c:v>
                 </c:pt>
-                <c:pt idx="14">
+                <c:pt idx="15">
                   <c:v>15</c:v>
                 </c:pt>
-                <c:pt idx="15">
+                <c:pt idx="16">
                   <c:v>16</c:v>
                 </c:pt>
-                <c:pt idx="16">
+                <c:pt idx="17">
                   <c:v>17</c:v>
                 </c:pt>
-                <c:pt idx="17">
+                <c:pt idx="18">
                   <c:v>18</c:v>
                 </c:pt>
-                <c:pt idx="18">
+                <c:pt idx="19">
                   <c:v>19</c:v>
                 </c:pt>
-                <c:pt idx="19">
+                <c:pt idx="20">
                   <c:v>20</c:v>
                 </c:pt>
               </c:numCache>
@@ -2836,35 +2834,37 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'10-Apr-11'!$O$7:$O$26</c:f>
+              <c:f>'10-Apr-11'!$O$6:$O$26</c:f>
               <c:numCache>
                 <c:formatCode>0.000</c:formatCode>
-                <c:ptCount val="20"/>
-                <c:pt idx="3">
-                  <c:v>6.3200000000000006E-2</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>0.2492</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>0.55380000000000007</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>0.97200000000000009</c:v>
-                </c:pt>
-                <c:pt idx="19">
+                <c:ptCount val="21"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.3</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.6</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.9</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>1.2</c:v>
+                </c:pt>
+                <c:pt idx="20">
                   <c:v>1.5</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
         </c:ser>
-        <c:dLbls/>
-        <c:axId val="81054336"/>
-        <c:axId val="73597696"/>
+        <c:axId val="88195072"/>
+        <c:axId val="88196992"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="81054336"/>
+        <c:axId val="88195072"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2890,12 +2890,12 @@
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="73597696"/>
+        <c:crossAx val="88196992"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="73597696"/>
+        <c:axId val="88196992"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2919,24 +2919,33 @@
           </c:tx>
           <c:layout/>
         </c:title>
-        <c:numFmt formatCode="0.00" sourceLinked="1"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="81054336"/>
+        <c:crossAx val="88195072"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.69890293203175613"/>
+          <c:y val="0.71407200291479889"/>
+          <c:w val="9.8207065019261269E-2"/>
+          <c:h val="9.9786129462100887E-2"/>
+        </c:manualLayout>
+      </c:layout>
     </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000244" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000244" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000255" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000255" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -2976,9 +2985,6 @@
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
-          <c:tx>
-            <c:v>Actual Flow Rate</c:v>
-          </c:tx>
           <c:trendline>
             <c:trendlineType val="linear"/>
             <c:dispRSqr val="1"/>
@@ -2986,7 +2992,7 @@
             <c:trendlineLbl>
               <c:layout>
                 <c:manualLayout>
-                  <c:x val="-0.10491973910986446"/>
+                  <c:x val="-0.10491973910986443"/>
                   <c:y val="-9.8167752954325706E-3"/>
                 </c:manualLayout>
               </c:layout>
@@ -2995,68 +3001,71 @@
           </c:trendline>
           <c:xVal>
             <c:numRef>
-              <c:f>'10-Apr-11 (2)'!$A$7:$A$26</c:f>
+              <c:f>'10-Apr-11 (2)'!$A$6:$A$26</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="20"/>
+                <c:ptCount val="21"/>
                 <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
                   <c:v>1</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="2">
                   <c:v>2</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="3">
                   <c:v>3</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="4">
                   <c:v>4</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="5">
                   <c:v>5</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="6">
                   <c:v>6</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="7">
                   <c:v>7</c:v>
                 </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="8">
                   <c:v>8</c:v>
                 </c:pt>
-                <c:pt idx="8">
+                <c:pt idx="9">
                   <c:v>9</c:v>
                 </c:pt>
-                <c:pt idx="9">
+                <c:pt idx="10">
                   <c:v>10</c:v>
                 </c:pt>
-                <c:pt idx="10">
+                <c:pt idx="11">
                   <c:v>11</c:v>
                 </c:pt>
-                <c:pt idx="11">
+                <c:pt idx="12">
                   <c:v>12</c:v>
                 </c:pt>
-                <c:pt idx="12">
+                <c:pt idx="13">
                   <c:v>13</c:v>
                 </c:pt>
-                <c:pt idx="13">
+                <c:pt idx="14">
                   <c:v>14</c:v>
                 </c:pt>
-                <c:pt idx="14">
+                <c:pt idx="15">
                   <c:v>15</c:v>
                 </c:pt>
-                <c:pt idx="15">
+                <c:pt idx="16">
                   <c:v>16</c:v>
                 </c:pt>
-                <c:pt idx="16">
+                <c:pt idx="17">
                   <c:v>17</c:v>
                 </c:pt>
-                <c:pt idx="17">
+                <c:pt idx="18">
                   <c:v>18</c:v>
                 </c:pt>
-                <c:pt idx="18">
+                <c:pt idx="19">
                   <c:v>19</c:v>
                 </c:pt>
-                <c:pt idx="19">
+                <c:pt idx="20">
                   <c:v>20</c:v>
                 </c:pt>
               </c:numCache>
@@ -3064,23 +3073,26 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'10-Apr-11 (2)'!$L$7:$L$26</c:f>
+              <c:f>'10-Apr-11 (2)'!$L$6:$L$26</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
-                <c:ptCount val="20"/>
-                <c:pt idx="3">
+                <c:ptCount val="21"/>
+                <c:pt idx="0" formatCode="General">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="4">
                   <c:v>0.31666666666666665</c:v>
                 </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="8">
                   <c:v>0.67222222222222228</c:v>
                 </c:pt>
-                <c:pt idx="11">
+                <c:pt idx="12">
                   <c:v>0.9277777777777777</c:v>
                 </c:pt>
-                <c:pt idx="15">
+                <c:pt idx="16">
                   <c:v>1.1944444444444444</c:v>
                 </c:pt>
-                <c:pt idx="19">
+                <c:pt idx="20">
                   <c:v>1.4444444444444444</c:v>
                 </c:pt>
               </c:numCache>
@@ -3090,73 +3102,73 @@
         <c:ser>
           <c:idx val="1"/>
           <c:order val="1"/>
-          <c:tx>
-            <c:v>Expected Flow Rate</c:v>
-          </c:tx>
           <c:xVal>
             <c:numRef>
-              <c:f>'10-Apr-11 (2)'!$A$7:$A$26</c:f>
+              <c:f>'10-Apr-11 (2)'!$A$6:$A$26</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="20"/>
+                <c:ptCount val="21"/>
                 <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
                   <c:v>1</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="2">
                   <c:v>2</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="3">
                   <c:v>3</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="4">
                   <c:v>4</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="5">
                   <c:v>5</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="6">
                   <c:v>6</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="7">
                   <c:v>7</c:v>
                 </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="8">
                   <c:v>8</c:v>
                 </c:pt>
-                <c:pt idx="8">
+                <c:pt idx="9">
                   <c:v>9</c:v>
                 </c:pt>
-                <c:pt idx="9">
+                <c:pt idx="10">
                   <c:v>10</c:v>
                 </c:pt>
-                <c:pt idx="10">
+                <c:pt idx="11">
                   <c:v>11</c:v>
                 </c:pt>
-                <c:pt idx="11">
+                <c:pt idx="12">
                   <c:v>12</c:v>
                 </c:pt>
-                <c:pt idx="12">
+                <c:pt idx="13">
                   <c:v>13</c:v>
                 </c:pt>
-                <c:pt idx="13">
+                <c:pt idx="14">
                   <c:v>14</c:v>
                 </c:pt>
-                <c:pt idx="14">
+                <c:pt idx="15">
                   <c:v>15</c:v>
                 </c:pt>
-                <c:pt idx="15">
+                <c:pt idx="16">
                   <c:v>16</c:v>
                 </c:pt>
-                <c:pt idx="16">
+                <c:pt idx="17">
                   <c:v>17</c:v>
                 </c:pt>
-                <c:pt idx="17">
+                <c:pt idx="18">
                   <c:v>18</c:v>
                 </c:pt>
-                <c:pt idx="18">
+                <c:pt idx="19">
                   <c:v>19</c:v>
                 </c:pt>
-                <c:pt idx="19">
+                <c:pt idx="20">
                   <c:v>20</c:v>
                 </c:pt>
               </c:numCache>
@@ -3164,23 +3176,26 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'10-Apr-11 (2)'!$D$7:$D$26</c:f>
+              <c:f>'10-Apr-11 (2)'!$D$6:$D$26</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="20"/>
-                <c:pt idx="3">
+                <c:ptCount val="21"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="4">
                   <c:v>0.317</c:v>
                 </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="8">
                   <c:v>0.624</c:v>
                 </c:pt>
-                <c:pt idx="11">
+                <c:pt idx="12">
                   <c:v>0.92400000000000004</c:v>
                 </c:pt>
-                <c:pt idx="15">
+                <c:pt idx="16">
                   <c:v>1.216</c:v>
                 </c:pt>
-                <c:pt idx="19">
+                <c:pt idx="20">
                   <c:v>1.5</c:v>
                 </c:pt>
               </c:numCache>
@@ -3190,76 +3205,73 @@
         <c:ser>
           <c:idx val="2"/>
           <c:order val="2"/>
-          <c:tx>
-            <c:v>Expected w/Multiplier</c:v>
-          </c:tx>
-          <c:trendline>
-            <c:trendlineType val="linear"/>
-          </c:trendline>
           <c:xVal>
             <c:numRef>
-              <c:f>'10-Apr-11 (2)'!$A$7:$A$26</c:f>
+              <c:f>'10-Apr-11 (2)'!$A$6:$A$26</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="20"/>
+                <c:ptCount val="21"/>
                 <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
                   <c:v>1</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="2">
                   <c:v>2</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="3">
                   <c:v>3</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="4">
                   <c:v>4</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="5">
                   <c:v>5</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="6">
                   <c:v>6</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="7">
                   <c:v>7</c:v>
                 </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="8">
                   <c:v>8</c:v>
                 </c:pt>
-                <c:pt idx="8">
+                <c:pt idx="9">
                   <c:v>9</c:v>
                 </c:pt>
-                <c:pt idx="9">
+                <c:pt idx="10">
                   <c:v>10</c:v>
                 </c:pt>
-                <c:pt idx="10">
+                <c:pt idx="11">
                   <c:v>11</c:v>
                 </c:pt>
-                <c:pt idx="11">
+                <c:pt idx="12">
                   <c:v>12</c:v>
                 </c:pt>
-                <c:pt idx="12">
+                <c:pt idx="13">
                   <c:v>13</c:v>
                 </c:pt>
-                <c:pt idx="13">
+                <c:pt idx="14">
                   <c:v>14</c:v>
                 </c:pt>
-                <c:pt idx="14">
+                <c:pt idx="15">
                   <c:v>15</c:v>
                 </c:pt>
-                <c:pt idx="15">
+                <c:pt idx="16">
                   <c:v>16</c:v>
                 </c:pt>
-                <c:pt idx="16">
+                <c:pt idx="17">
                   <c:v>17</c:v>
                 </c:pt>
-                <c:pt idx="17">
+                <c:pt idx="18">
                   <c:v>18</c:v>
                 </c:pt>
-                <c:pt idx="18">
+                <c:pt idx="19">
                   <c:v>19</c:v>
                 </c:pt>
-                <c:pt idx="19">
+                <c:pt idx="20">
                   <c:v>20</c:v>
                 </c:pt>
               </c:numCache>
@@ -3267,35 +3279,37 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'10-Apr-11 (2)'!$P$7:$P$26</c:f>
+              <c:f>'10-Apr-11 (2)'!$O$6:$O$26</c:f>
               <c:numCache>
                 <c:formatCode>0.000</c:formatCode>
-                <c:ptCount val="20"/>
-                <c:pt idx="3">
-                  <c:v>-0.2533333333333333</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>-0.40333333333333338</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>-0.37111111111111106</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>-0.23888888888888893</c:v>
-                </c:pt>
-                <c:pt idx="19">
+                <c:ptCount val="21"/>
+                <c:pt idx="0">
                   <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.28888888888888886</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.57777777777777772</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.86666666666666659</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>1.1555555555555554</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>1.4444444444444444</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
         </c:ser>
-        <c:dLbls/>
-        <c:axId val="81151488"/>
-        <c:axId val="81153408"/>
+        <c:axId val="90532480"/>
+        <c:axId val="90542848"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="81151488"/>
+        <c:axId val="90532480"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3321,12 +3335,12 @@
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="81153408"/>
+        <c:crossAx val="90542848"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="81153408"/>
+        <c:axId val="90542848"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3350,10 +3364,10 @@
           </c:tx>
           <c:layout/>
         </c:title>
-        <c:numFmt formatCode="0.00" sourceLinked="1"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="81151488"/>
+        <c:crossAx val="90532480"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3367,7 +3381,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000266" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000266" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000278" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000278" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -3558,10 +3572,10 @@
       <xdr:rowOff>114300</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>1076325</xdr:colOff>
-      <xdr:row>48</xdr:row>
-      <xdr:rowOff>95250</xdr:rowOff>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>771525</xdr:colOff>
+      <xdr:row>52</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -6779,8 +6793,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:S26"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="T20" sqref="T20"/>
+    <sheetView tabSelected="1" topLeftCell="A32" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="O11" sqref="O11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -6842,10 +6856,10 @@
         <v>28</v>
       </c>
       <c r="O4" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="R4" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="5" spans="1:19">
@@ -6890,24 +6904,26 @@
       </c>
       <c r="N5" s="7"/>
       <c r="O5" s="7" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="P5" s="7" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="Q5" s="17"/>
       <c r="R5" s="7" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="S5" s="7" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
     </row>
     <row r="6" spans="1:19">
       <c r="A6" s="25">
         <v>0</v>
       </c>
-      <c r="B6" s="25"/>
+      <c r="B6" s="6">
+        <v>60</v>
+      </c>
       <c r="C6" s="26"/>
       <c r="D6" s="29">
         <v>0</v>
@@ -6939,7 +6955,7 @@
       <c r="M6" s="17"/>
       <c r="N6" s="17"/>
       <c r="O6" s="41">
-        <f>D6*A6/$A$26</f>
+        <f>$D$26*A6/$A$26</f>
         <v>0</v>
       </c>
       <c r="P6" s="39">
@@ -6959,9 +6975,6 @@
     <row r="7" spans="1:19">
       <c r="A7" s="6">
         <v>1</v>
-      </c>
-      <c r="B7" s="6">
-        <v>60</v>
       </c>
       <c r="C7" s="6"/>
       <c r="D7" s="24"/>
@@ -6973,9 +6986,7 @@
       <c r="J7" s="8"/>
       <c r="K7" s="19"/>
       <c r="L7" s="22"/>
-      <c r="M7" s="8">
-        <v>0</v>
-      </c>
+      <c r="M7" s="8"/>
       <c r="N7" s="16"/>
       <c r="O7" s="41"/>
       <c r="P7" s="39"/>
@@ -7048,14 +7059,14 @@
         <v>18</v>
       </c>
       <c r="H10" s="8">
-        <f t="shared" ref="H7:H26" si="1">G10/B10</f>
+        <f t="shared" ref="H10:H26" si="1">G10/B10</f>
         <v>0.3</v>
       </c>
       <c r="I10" s="8">
         <v>19</v>
       </c>
       <c r="J10" s="8">
-        <f t="shared" ref="J7:J22" si="2">I10/B10</f>
+        <f t="shared" ref="J10:J22" si="2">I10/B10</f>
         <v>0.31666666666666665</v>
       </c>
       <c r="K10" s="19">
@@ -7072,19 +7083,19 @@
       </c>
       <c r="N10" s="14"/>
       <c r="O10" s="41">
-        <f t="shared" ref="O7:O26" si="5">D10*A10/$A$26</f>
-        <v>6.3200000000000006E-2</v>
+        <f t="shared" ref="O7:O26" si="5">$D$26*A10/$A$26</f>
+        <v>0.3</v>
       </c>
       <c r="P10" s="39">
-        <f t="shared" ref="P7:P26" si="6">O10-D10</f>
-        <v>-0.25280000000000002</v>
+        <f t="shared" ref="P10:P26" si="6">O10-D10</f>
+        <v>-1.6000000000000014E-2</v>
       </c>
       <c r="R10" s="41">
-        <f t="shared" ref="R7:R26" si="7">L10*A10/$A$26</f>
+        <f t="shared" ref="R10:R22" si="7">L10*A10/$A$26</f>
         <v>6.222222222222222E-2</v>
       </c>
       <c r="S10" s="39">
-        <f t="shared" ref="S7:S26" si="8">R10-L10</f>
+        <f t="shared" ref="S10:S26" si="8">R10-L10</f>
         <v>-0.24888888888888888</v>
       </c>
     </row>
@@ -7105,7 +7116,7 @@
       <c r="L11" s="22"/>
       <c r="M11" s="8"/>
       <c r="N11" s="14"/>
-      <c r="O11" s="41"/>
+      <c r="O11" s="45"/>
       <c r="P11" s="39"/>
       <c r="R11" s="41"/>
       <c r="S11" s="39"/>
@@ -7201,11 +7212,11 @@
       <c r="N14" s="38"/>
       <c r="O14" s="42">
         <f t="shared" si="5"/>
-        <v>0.2492</v>
+        <v>0.6</v>
       </c>
       <c r="P14" s="40">
         <f t="shared" si="6"/>
-        <v>-0.37380000000000002</v>
+        <v>-2.300000000000002E-2</v>
       </c>
       <c r="Q14" s="36"/>
       <c r="R14" s="42">
@@ -7330,11 +7341,11 @@
       <c r="N18" s="14"/>
       <c r="O18" s="41">
         <f t="shared" si="5"/>
-        <v>0.55380000000000007</v>
+        <v>0.9</v>
       </c>
       <c r="P18" s="39">
         <f t="shared" si="6"/>
-        <v>-0.36919999999999997</v>
+        <v>-2.300000000000002E-2</v>
       </c>
       <c r="R18" s="41">
         <f t="shared" si="7"/>
@@ -7458,11 +7469,11 @@
       <c r="N22" s="14"/>
       <c r="O22" s="41">
         <f t="shared" si="5"/>
-        <v>0.97200000000000009</v>
+        <v>1.2</v>
       </c>
       <c r="P22" s="39">
         <f t="shared" si="6"/>
-        <v>-0.24299999999999999</v>
+        <v>-1.5000000000000124E-2</v>
       </c>
       <c r="R22" s="41">
         <f t="shared" si="7"/>
@@ -7613,10 +7624,11 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:Q27"/>
+  <dimension ref="A1:R27"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="Q26" sqref="Q26"/>
+    <sheetView workbookViewId="0">
+      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="P23" sqref="P23:P24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -7627,14 +7639,14 @@
     <col min="5" max="5" width="25.85546875" customWidth="1"/>
     <col min="6" max="10" width="24.140625" customWidth="1"/>
     <col min="11" max="11" width="25" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="24.140625" customWidth="1"/>
+    <col min="12" max="12" width="25.85546875" customWidth="1"/>
     <col min="13" max="13" width="14.28515625" customWidth="1"/>
     <col min="15" max="15" width="13" customWidth="1"/>
     <col min="16" max="16" width="12.85546875" customWidth="1"/>
     <col min="17" max="17" width="12.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17">
+    <row r="1" spans="1:18">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -7651,7 +7663,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:17">
+    <row r="2" spans="1:18">
       <c r="A2" s="2">
         <v>40643</v>
       </c>
@@ -7659,7 +7671,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:17">
+    <row r="3" spans="1:18">
       <c r="A3" s="3">
         <v>2.9166666666666664E-2</v>
       </c>
@@ -7667,7 +7679,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="4" spans="1:17">
+    <row r="4" spans="1:18">
       <c r="E4" t="s">
         <v>26</v>
       </c>
@@ -7677,8 +7689,14 @@
       <c r="I4" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="5" spans="1:17">
+      <c r="O4" t="s">
+        <v>34</v>
+      </c>
+      <c r="Q4" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="5" spans="1:18">
       <c r="A5" s="5" t="s">
         <v>1</v>
       </c>
@@ -7719,14 +7737,19 @@
         <v>5</v>
       </c>
       <c r="O5" s="7" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="P5" s="7" t="s">
-        <v>32</v>
-      </c>
-      <c r="Q5" s="17"/>
-    </row>
-    <row r="6" spans="1:17">
+        <v>30</v>
+      </c>
+      <c r="Q5" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="R5" s="7" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="6" spans="1:18">
       <c r="A6" s="27">
         <v>0</v>
       </c>
@@ -7765,16 +7788,23 @@
         <v>0</v>
       </c>
       <c r="O6" s="32">
-        <f>L6*A6/$A$26</f>
+        <f>$L$26*A6/$A$26</f>
         <v>0</v>
       </c>
       <c r="P6" s="32">
         <f>O6-L6</f>
         <v>0</v>
       </c>
-      <c r="Q6" s="17"/>
-    </row>
-    <row r="7" spans="1:17">
+      <c r="Q6" s="32">
+        <f>$D$26*A6/$A$26</f>
+        <v>0</v>
+      </c>
+      <c r="R6" s="32">
+        <f>Q6-D6</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:18">
       <c r="A7" s="6">
         <v>1</v>
       </c>
@@ -7790,13 +7820,12 @@
       <c r="K7" s="19"/>
       <c r="L7" s="22"/>
       <c r="M7" s="8"/>
-      <c r="O7" s="32">
-        <f t="shared" ref="O7:O26" si="0">L7*A7/$A$26</f>
-        <v>0</v>
-      </c>
+      <c r="O7" s="32"/>
       <c r="P7" s="32"/>
-    </row>
-    <row r="8" spans="1:17" ht="12.75" customHeight="1">
+      <c r="Q7" s="32"/>
+      <c r="R7" s="32"/>
+    </row>
+    <row r="8" spans="1:18" ht="12.75" customHeight="1">
       <c r="A8" s="6">
         <v>2</v>
       </c>
@@ -7812,13 +7841,12 @@
       <c r="K8" s="19"/>
       <c r="L8" s="22"/>
       <c r="M8" s="8"/>
-      <c r="O8" s="32">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
+      <c r="O8" s="32"/>
       <c r="P8" s="32"/>
-    </row>
-    <row r="9" spans="1:17">
+      <c r="Q8" s="32"/>
+      <c r="R8" s="32"/>
+    </row>
+    <row r="9" spans="1:18">
       <c r="A9" s="6">
         <v>3</v>
       </c>
@@ -7834,13 +7862,12 @@
       <c r="K9" s="19"/>
       <c r="L9" s="22"/>
       <c r="M9" s="8"/>
-      <c r="O9" s="32">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
+      <c r="O9" s="32"/>
       <c r="P9" s="32"/>
-    </row>
-    <row r="10" spans="1:17">
+      <c r="Q9" s="32"/>
+      <c r="R9" s="32"/>
+    </row>
+    <row r="10" spans="1:18">
       <c r="A10" s="6">
         <v>4</v>
       </c>
@@ -7855,29 +7882,29 @@
         <v>18</v>
       </c>
       <c r="F10" s="8">
-        <f t="shared" ref="F10:F26" si="1">E10/B10</f>
+        <f t="shared" ref="F10:F26" si="0">E10/B10</f>
         <v>0.3</v>
       </c>
       <c r="G10" s="8">
         <v>19</v>
       </c>
       <c r="H10" s="8">
-        <f t="shared" ref="H7:H26" si="2">G10/B10</f>
+        <f t="shared" ref="H10:H26" si="1">G10/B10</f>
         <v>0.31666666666666665</v>
       </c>
       <c r="I10" s="8">
         <v>20</v>
       </c>
       <c r="J10" s="8">
-        <f t="shared" ref="J10" si="3">I10/B10</f>
+        <f t="shared" ref="J10" si="2">I10/B10</f>
         <v>0.33333333333333331</v>
       </c>
       <c r="K10" s="19">
-        <f t="shared" ref="K10:K26" si="4">AVERAGE(E10,G10,I10)</f>
+        <f t="shared" ref="K10:K26" si="3">AVERAGE(E10,G10,I10)</f>
         <v>19</v>
       </c>
       <c r="L10" s="22">
-        <f t="shared" ref="L10:L26" si="5">K10/B10</f>
+        <f t="shared" ref="L10:L26" si="4">K10/B10</f>
         <v>0.31666666666666665</v>
       </c>
       <c r="M10" s="8">
@@ -7885,15 +7912,23 @@
         <v>0.11111111111111738</v>
       </c>
       <c r="O10" s="32">
-        <f t="shared" si="0"/>
-        <v>6.3333333333333325E-2</v>
+        <f t="shared" ref="O7:O26" si="5">$L$26*A10/$A$26</f>
+        <v>0.28888888888888886</v>
       </c>
       <c r="P10" s="32">
-        <f t="shared" ref="P7:P26" si="6">O10-L10</f>
-        <v>-0.2533333333333333</v>
-      </c>
-    </row>
-    <row r="11" spans="1:17">
+        <f t="shared" ref="P10:P26" si="6">O10-L10</f>
+        <v>-2.777777777777779E-2</v>
+      </c>
+      <c r="Q10" s="32">
+        <f t="shared" ref="Q7:Q26" si="7">$D$26*A10/$A$26</f>
+        <v>0.3</v>
+      </c>
+      <c r="R10" s="32">
+        <f t="shared" ref="R7:R26" si="8">Q10-D10</f>
+        <v>-1.7000000000000015E-2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:18">
       <c r="A11" s="6">
         <v>5</v>
       </c>
@@ -7909,13 +7944,12 @@
       <c r="K11" s="19"/>
       <c r="L11" s="22"/>
       <c r="M11" s="8"/>
-      <c r="O11" s="32">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
+      <c r="O11" s="32"/>
       <c r="P11" s="32"/>
-    </row>
-    <row r="12" spans="1:17">
+      <c r="Q11" s="32"/>
+      <c r="R11" s="32"/>
+    </row>
+    <row r="12" spans="1:18">
       <c r="A12" s="6">
         <v>6</v>
       </c>
@@ -7931,13 +7965,12 @@
       <c r="K12" s="19"/>
       <c r="L12" s="22"/>
       <c r="M12" s="8"/>
-      <c r="O12" s="32">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
+      <c r="O12" s="32"/>
       <c r="P12" s="32"/>
-    </row>
-    <row r="13" spans="1:17">
+      <c r="Q12" s="32"/>
+      <c r="R12" s="32"/>
+    </row>
+    <row r="13" spans="1:18">
       <c r="A13" s="6">
         <v>7</v>
       </c>
@@ -7953,67 +7986,74 @@
       <c r="K13" s="19"/>
       <c r="L13" s="22"/>
       <c r="M13" s="8"/>
-      <c r="O13" s="32">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
+      <c r="O13" s="32"/>
       <c r="P13" s="32"/>
-    </row>
-    <row r="14" spans="1:17">
+      <c r="Q13" s="32"/>
+      <c r="R13" s="32"/>
+    </row>
+    <row r="14" spans="1:18">
       <c r="A14" s="33">
         <v>8</v>
       </c>
-      <c r="B14" s="33">
+      <c r="B14" s="20">
         <v>60</v>
       </c>
-      <c r="C14" s="33"/>
-      <c r="D14" s="33">
+      <c r="C14" s="20"/>
+      <c r="D14" s="24">
         <v>0.624</v>
       </c>
-      <c r="E14" s="34">
+      <c r="E14" s="18">
         <v>38</v>
       </c>
-      <c r="F14" s="35">
+      <c r="F14" s="19">
+        <f t="shared" si="0"/>
+        <v>0.6333333333333333</v>
+      </c>
+      <c r="G14" s="19">
+        <v>38</v>
+      </c>
+      <c r="H14" s="19">
         <f t="shared" si="1"/>
         <v>0.6333333333333333</v>
       </c>
-      <c r="G14" s="35">
-        <v>38</v>
-      </c>
-      <c r="H14" s="35">
-        <f t="shared" si="2"/>
-        <v>0.6333333333333333</v>
-      </c>
-      <c r="I14" s="35">
+      <c r="I14" s="19">
         <v>45</v>
       </c>
-      <c r="J14" s="35">
+      <c r="J14" s="19">
         <f>I14/70</f>
         <v>0.6428571428571429</v>
       </c>
-      <c r="K14" s="35">
+      <c r="K14" s="19">
+        <f t="shared" si="3"/>
+        <v>40.333333333333336</v>
+      </c>
+      <c r="L14" s="22">
         <f t="shared" si="4"/>
-        <v>40.333333333333336</v>
-      </c>
-      <c r="L14" s="35">
+        <v>0.67222222222222228</v>
+      </c>
+      <c r="M14" s="19">
+        <f t="shared" ref="M14:M26" si="9">((D14-L14)/F14)*100</f>
+        <v>-7.6140350877193077</v>
+      </c>
+      <c r="N14" s="43"/>
+      <c r="O14" s="44">
         <f t="shared" si="5"/>
-        <v>0.67222222222222228</v>
-      </c>
-      <c r="M14" s="35">
-        <f t="shared" ref="M14:M26" si="7">((D14-L14)/F14)*100</f>
-        <v>-7.6140350877193077</v>
-      </c>
-      <c r="N14" s="36"/>
-      <c r="O14" s="37">
-        <f t="shared" si="0"/>
-        <v>0.2688888888888889</v>
+        <v>0.57777777777777772</v>
       </c>
       <c r="P14" s="37">
-        <f t="shared" si="6"/>
-        <v>-0.40333333333333338</v>
-      </c>
-    </row>
-    <row r="15" spans="1:17">
+        <f>O14-L14</f>
+        <v>-9.4444444444444553E-2</v>
+      </c>
+      <c r="Q14" s="44">
+        <f t="shared" si="7"/>
+        <v>0.6</v>
+      </c>
+      <c r="R14" s="37">
+        <f t="shared" si="8"/>
+        <v>-2.4000000000000021E-2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:18">
       <c r="A15" s="6">
         <v>9</v>
       </c>
@@ -8029,13 +8069,12 @@
       <c r="K15" s="19"/>
       <c r="L15" s="22"/>
       <c r="M15" s="8"/>
-      <c r="O15" s="32">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
+      <c r="O15" s="32"/>
       <c r="P15" s="32"/>
-    </row>
-    <row r="16" spans="1:17">
+      <c r="Q15" s="32"/>
+      <c r="R15" s="32"/>
+    </row>
+    <row r="16" spans="1:18">
       <c r="A16" s="6">
         <v>10</v>
       </c>
@@ -8051,13 +8090,12 @@
       <c r="K16" s="19"/>
       <c r="L16" s="22"/>
       <c r="M16" s="8"/>
-      <c r="O16" s="32">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
+      <c r="O16" s="32"/>
       <c r="P16" s="32"/>
-    </row>
-    <row r="17" spans="1:16">
+      <c r="Q16" s="32"/>
+      <c r="R16" s="32"/>
+    </row>
+    <row r="17" spans="1:18">
       <c r="A17" s="6">
         <v>11</v>
       </c>
@@ -8073,14 +8111,13 @@
       <c r="K17" s="19"/>
       <c r="L17" s="22"/>
       <c r="M17" s="8"/>
-      <c r="O17" s="32">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
+      <c r="O17" s="32"/>
       <c r="P17" s="32"/>
-    </row>
-    <row r="18" spans="1:16">
-      <c r="A18" s="6">
+      <c r="Q17" s="32"/>
+      <c r="R17" s="32"/>
+    </row>
+    <row r="18" spans="1:18">
+      <c r="A18" s="33">
         <v>12</v>
       </c>
       <c r="B18" s="6">
@@ -8094,14 +8131,14 @@
         <v>56</v>
       </c>
       <c r="F18" s="8">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0.93333333333333335</v>
       </c>
       <c r="G18" s="8">
         <v>55</v>
       </c>
       <c r="H18" s="8">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>0.91666666666666663</v>
       </c>
       <c r="I18" s="8">
@@ -8112,27 +8149,35 @@
         <v>0.93333333333333335</v>
       </c>
       <c r="K18" s="19">
+        <f t="shared" si="3"/>
+        <v>55.666666666666664</v>
+      </c>
+      <c r="L18" s="22">
         <f t="shared" si="4"/>
-        <v>55.666666666666664</v>
-      </c>
-      <c r="L18" s="22">
+        <v>0.9277777777777777</v>
+      </c>
+      <c r="M18" s="8">
+        <f t="shared" si="9"/>
+        <v>-0.40476190476189189</v>
+      </c>
+      <c r="O18" s="32">
         <f t="shared" si="5"/>
-        <v>0.9277777777777777</v>
-      </c>
-      <c r="M18" s="8">
-        <f t="shared" si="7"/>
-        <v>-0.40476190476189189</v>
-      </c>
-      <c r="O18" s="32">
-        <f t="shared" si="0"/>
-        <v>0.55666666666666664</v>
+        <v>0.86666666666666659</v>
       </c>
       <c r="P18" s="32">
         <f t="shared" si="6"/>
-        <v>-0.37111111111111106</v>
-      </c>
-    </row>
-    <row r="19" spans="1:16">
+        <v>-6.1111111111111116E-2</v>
+      </c>
+      <c r="Q18" s="32">
+        <f t="shared" si="7"/>
+        <v>0.9</v>
+      </c>
+      <c r="R18" s="37">
+        <f t="shared" si="8"/>
+        <v>-2.4000000000000021E-2</v>
+      </c>
+    </row>
+    <row r="19" spans="1:18">
       <c r="A19" s="6">
         <v>13</v>
       </c>
@@ -8148,13 +8193,12 @@
       <c r="K19" s="19"/>
       <c r="L19" s="22"/>
       <c r="M19" s="8"/>
-      <c r="O19" s="32">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
+      <c r="O19" s="32"/>
       <c r="P19" s="32"/>
-    </row>
-    <row r="20" spans="1:16">
+      <c r="Q19" s="32"/>
+      <c r="R19" s="32"/>
+    </row>
+    <row r="20" spans="1:18">
       <c r="A20" s="6">
         <v>14</v>
       </c>
@@ -8170,13 +8214,12 @@
       <c r="K20" s="19"/>
       <c r="L20" s="22"/>
       <c r="M20" s="8"/>
-      <c r="O20" s="32">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
+      <c r="O20" s="32"/>
       <c r="P20" s="32"/>
-    </row>
-    <row r="21" spans="1:16">
+      <c r="Q20" s="32"/>
+      <c r="R20" s="32"/>
+    </row>
+    <row r="21" spans="1:18">
       <c r="A21" s="6">
         <v>15</v>
       </c>
@@ -8192,13 +8235,12 @@
       <c r="K21" s="19"/>
       <c r="L21" s="22"/>
       <c r="M21" s="8"/>
-      <c r="O21" s="32">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
+      <c r="O21" s="32"/>
       <c r="P21" s="32"/>
-    </row>
-    <row r="22" spans="1:16">
+      <c r="Q21" s="32"/>
+      <c r="R21" s="32"/>
+    </row>
+    <row r="22" spans="1:18">
       <c r="A22" s="6">
         <v>16</v>
       </c>
@@ -8213,45 +8255,53 @@
         <v>71</v>
       </c>
       <c r="F22" s="8">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>1.1833333333333333</v>
       </c>
       <c r="G22" s="8">
         <v>72</v>
       </c>
       <c r="H22" s="8">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>1.2</v>
       </c>
       <c r="I22" s="8">
         <v>72</v>
       </c>
       <c r="J22" s="8">
-        <f t="shared" ref="J22:J26" si="8">I22/B22</f>
+        <f t="shared" ref="J22:J26" si="10">I22/B22</f>
         <v>1.2</v>
       </c>
       <c r="K22" s="19">
+        <f t="shared" si="3"/>
+        <v>71.666666666666671</v>
+      </c>
+      <c r="L22" s="22">
         <f t="shared" si="4"/>
-        <v>71.666666666666671</v>
-      </c>
-      <c r="L22" s="22">
+        <v>1.1944444444444444</v>
+      </c>
+      <c r="M22" s="8">
+        <f t="shared" si="9"/>
+        <v>1.821596244131455</v>
+      </c>
+      <c r="O22" s="32">
         <f t="shared" si="5"/>
-        <v>1.1944444444444444</v>
-      </c>
-      <c r="M22" s="8">
-        <f t="shared" si="7"/>
-        <v>1.821596244131455</v>
-      </c>
-      <c r="O22" s="32">
-        <f t="shared" si="0"/>
-        <v>0.95555555555555549</v>
+        <v>1.1555555555555554</v>
       </c>
       <c r="P22" s="32">
         <f t="shared" si="6"/>
-        <v>-0.23888888888888893</v>
-      </c>
-    </row>
-    <row r="23" spans="1:16">
+        <v>-3.8888888888888973E-2</v>
+      </c>
+      <c r="Q22" s="32">
+        <f t="shared" si="7"/>
+        <v>1.2</v>
+      </c>
+      <c r="R22" s="32">
+        <f t="shared" si="8"/>
+        <v>-1.6000000000000014E-2</v>
+      </c>
+    </row>
+    <row r="23" spans="1:18">
       <c r="A23" s="6">
         <v>17</v>
       </c>
@@ -8267,13 +8317,12 @@
       <c r="K23" s="19"/>
       <c r="L23" s="22"/>
       <c r="M23" s="8"/>
-      <c r="O23" s="32">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
+      <c r="O23" s="32"/>
       <c r="P23" s="32"/>
-    </row>
-    <row r="24" spans="1:16">
+      <c r="Q23" s="32"/>
+      <c r="R23" s="32"/>
+    </row>
+    <row r="24" spans="1:18">
       <c r="A24" s="6">
         <v>18</v>
       </c>
@@ -8289,13 +8338,12 @@
       <c r="K24" s="19"/>
       <c r="L24" s="22"/>
       <c r="M24" s="8"/>
-      <c r="O24" s="32">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
+      <c r="O24" s="32"/>
       <c r="P24" s="32"/>
-    </row>
-    <row r="25" spans="1:16">
+      <c r="Q24" s="32"/>
+      <c r="R24" s="32"/>
+    </row>
+    <row r="25" spans="1:18">
       <c r="A25" s="6">
         <v>19</v>
       </c>
@@ -8311,13 +8359,12 @@
       <c r="K25" s="19"/>
       <c r="L25" s="22"/>
       <c r="M25" s="8"/>
-      <c r="O25" s="32">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
+      <c r="O25" s="32"/>
       <c r="P25" s="32"/>
-    </row>
-    <row r="26" spans="1:16">
+      <c r="Q25" s="32"/>
+      <c r="R25" s="32"/>
+    </row>
+    <row r="26" spans="1:18">
       <c r="A26" s="6">
         <v>20</v>
       </c>
@@ -8335,45 +8382,53 @@
         <v>86</v>
       </c>
       <c r="F26" s="8">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>1.4333333333333333</v>
       </c>
       <c r="G26" s="8">
         <v>87</v>
       </c>
       <c r="H26" s="8">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>1.45</v>
       </c>
       <c r="I26" s="8">
         <v>87</v>
       </c>
       <c r="J26" s="8">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>1.45</v>
       </c>
       <c r="K26" s="19">
+        <f t="shared" si="3"/>
+        <v>86.666666666666671</v>
+      </c>
+      <c r="L26" s="22">
         <f t="shared" si="4"/>
-        <v>86.666666666666671</v>
-      </c>
-      <c r="L26" s="22">
+        <v>1.4444444444444444</v>
+      </c>
+      <c r="M26" s="8">
+        <f t="shared" si="9"/>
+        <v>3.875968992248064</v>
+      </c>
+      <c r="O26" s="32">
         <f t="shared" si="5"/>
-        <v>1.4444444444444444</v>
-      </c>
-      <c r="M26" s="8">
-        <f t="shared" si="7"/>
-        <v>3.875968992248064</v>
-      </c>
-      <c r="O26" s="32">
-        <f>L26*A26/$A$26</f>
         <v>1.4444444444444444</v>
       </c>
       <c r="P26" s="32">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="27" spans="1:16">
+      <c r="Q26" s="32">
+        <f t="shared" si="7"/>
+        <v>1.5</v>
+      </c>
+      <c r="R26" s="32">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:18">
       <c r="N27" s="14"/>
       <c r="O27" s="14"/>
     </row>
@@ -8382,33 +8437,4 @@
   <pageSetup orientation="portrait" r:id="rId1"/>
   <drawing r:id="rId2"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <cols>
-    <col min="1" max="1" width="10.7109375" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:4">
-      <c r="A1" t="s">
-        <v>30</v>
-      </c>
-      <c r="B1" t="s">
-        <v>31</v>
-      </c>
-      <c r="D1" t="s">
-        <v>32</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>